<commit_message>
works with ll table
</commit_message>
<xml_diff>
--- a/Методы компиляции.xlsx
+++ b/Методы компиляции.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Лабораторные работы\Семестр 6\Методы компиляции\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6DE3B9-BF67-4DE6-9940-D5F8B0CB365C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55EE599-775E-48AB-A643-DAFCE22081AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{79D62930-72F9-4DD1-8E2B-F1E1775E3F45}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="188">
   <si>
     <t>буква</t>
   </si>
@@ -822,7 +822,54 @@
     <t>С</t>
   </si>
   <si>
-    <t>C — равно/оператор сравнения</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Комментарий</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <r>
+      <t>F</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — комментарий</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — / или //</t>
+    </r>
+  </si>
+  <si>
+    <t>F/30</t>
+  </si>
+  <si>
+    <t>C — = или ==</t>
+  </si>
+  <si>
+    <t>E/22</t>
   </si>
 </sst>
 </file>
@@ -895,7 +942,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -908,12 +955,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1230,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CA9F56D-F00E-4794-B681-57966BFBA237}">
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1336,7 +1382,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>180</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>27</v>
@@ -1478,7 +1524,7 @@
         <v>46</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
@@ -1557,7 +1603,7 @@
         <v>46</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
@@ -1641,229 +1687,397 @@
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
     </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="T6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="W6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="X6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="7" spans="1:27">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y7" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T9" s="1" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27">
-      <c r="A8" s="5">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="5">
-        <v>11</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L8" s="5">
-        <v>21</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="T8" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27">
-      <c r="A9" s="5">
-        <v>1</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="5">
-        <v>12</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L9" s="5">
-        <v>22</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="T9" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:27">
       <c r="A10" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G10" s="5">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L10" s="5">
-        <v>23</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="M10" s="5">
+        <v>21</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G11" s="5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="5">
-        <v>24</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="T11" s="9" t="s">
-        <v>180</v>
+        <v>67</v>
+      </c>
+      <c r="M11" s="5">
+        <v>22</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G12" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="5">
-        <v>25</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="T12" s="9" t="s">
-        <v>91</v>
+        <v>68</v>
+      </c>
+      <c r="M12" s="5">
+        <v>23</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G13" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="L13" s="5">
-        <v>26</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="T13" s="9" t="s">
-        <v>92</v>
+        <v>69</v>
+      </c>
+      <c r="M13" s="5">
+        <v>24</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="5">
-        <v>27</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="M14" s="5">
+        <v>25</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G15" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L15" s="5">
-        <v>28</v>
-      </c>
-      <c r="M15" s="5" t="s">
-        <v>82</v>
+        <v>71</v>
+      </c>
+      <c r="M15" s="5">
+        <v>26</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:27">
       <c r="A16" s="5">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="5">
+        <v>17</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="M16" s="5">
+        <v>27</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="5">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="5">
+        <v>18</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M17" s="5">
+        <v>28</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="5">
         <v>9</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G18" s="5">
         <v>19</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="L16" s="5">
+      <c r="M18" s="5">
         <v>29</v>
       </c>
-      <c r="M16" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="T16" s="8"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="5">
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="5">
         <v>10</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G19" s="5">
         <v>20</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>74</v>
       </c>
+      <c r="M19" s="5">
+        <v>30</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="M20" s="5"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="5"/>

</xml_diff>